<commit_message>
fixed iE issue with appium dependency
</commit_message>
<xml_diff>
--- a/VTBCapital/TestData/MASTERSHEET.xlsx
+++ b/VTBCapital/TestData/MASTERSHEET.xlsx
@@ -588,7 +588,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -599,7 +599,7 @@
   <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -996,7 +996,7 @@
         <v>56</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>45</v>
+        <v>16</v>
       </c>
       <c r="D20" s="3" t="s">
         <v>52</v>
@@ -1016,7 +1016,7 @@
         <v>49</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>45</v>
+        <v>16</v>
       </c>
       <c r="D21" s="3" t="s">
         <v>52</v>

</xml_diff>

<commit_message>
mergin with Nitish's changes
</commit_message>
<xml_diff>
--- a/VTBCapital/TestData/MASTERSHEET.xlsx
+++ b/VTBCapital/TestData/MASTERSHEET.xlsx
@@ -168,12 +168,6 @@
     <t>TC_1021</t>
   </si>
   <si>
-    <t>Individual Account for Existing Customer having Joint Account Only(Flow3)</t>
-  </si>
-  <si>
-    <t>Joint Account for both Existing Customers(Flow5)</t>
-  </si>
-  <si>
     <t>Joint Account for both New Customers(Flow4)</t>
   </si>
   <si>
@@ -189,10 +183,16 @@
     <t>Test Case Description</t>
   </si>
   <si>
-    <t>Joint Account for One New and One Existing Customer(Flow7)</t>
-  </si>
-  <si>
     <t>Individual Account for New Customer</t>
+  </si>
+  <si>
+    <t>Joint Account for One New and One Existing Customer</t>
+  </si>
+  <si>
+    <t>Individual Account for Existing Customer having Joint Account Only</t>
+  </si>
+  <si>
+    <t>Joint Account for both Existing Customers</t>
   </si>
 </sst>
 </file>
@@ -588,7 +588,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -599,7 +599,7 @@
   <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -633,19 +633,19 @@
         <v>26</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>45</v>
+        <v>16</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>6</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -653,19 +653,19 @@
         <v>27</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>16</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>7</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -673,19 +673,19 @@
         <v>28</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>16</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>8</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -693,19 +693,19 @@
         <v>29</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>16</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>9</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -713,19 +713,19 @@
         <v>30</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>16</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>10</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -733,19 +733,19 @@
         <v>31</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>16</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E7" s="3" t="s">
         <v>11</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -753,19 +753,19 @@
         <v>32</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>16</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E8" s="3" t="s">
         <v>12</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -773,19 +773,19 @@
         <v>33</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>16</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E9" s="3" t="s">
         <v>13</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -793,19 +793,19 @@
         <v>34</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>16</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>14</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -813,19 +813,19 @@
         <v>35</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>16</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E11" s="3" t="s">
         <v>15</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -833,19 +833,19 @@
         <v>36</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>16</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E12" s="3" t="s">
         <v>17</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -853,19 +853,19 @@
         <v>37</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>16</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E13" s="3" t="s">
         <v>18</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -873,19 +873,19 @@
         <v>38</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>16</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E14" s="3" t="s">
         <v>19</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -893,19 +893,19 @@
         <v>39</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>16</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E15" s="3" t="s">
         <v>20</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -913,19 +913,19 @@
         <v>40</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>16</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E16" s="3" t="s">
         <v>21</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -933,19 +933,19 @@
         <v>41</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>16</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E17" s="3" t="s">
         <v>22</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -953,19 +953,19 @@
         <v>42</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>16</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E18" s="3" t="s">
         <v>23</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -973,19 +973,19 @@
         <v>43</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C19" s="3" t="s">
         <v>16</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E19" s="3" t="s">
         <v>24</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -993,19 +993,19 @@
         <v>44</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>16</v>
+        <v>45</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E20" s="3" t="s">
         <v>25</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
@@ -1013,19 +1013,19 @@
         <v>46</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>48</v>
+        <v>55</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>16</v>
+        <v>45</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E21" s="3" t="s">
         <v>25</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
@@ -1033,19 +1033,19 @@
         <v>47</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="C22" s="3" t="s">
         <v>16</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E22" s="3" t="s">
         <v>25</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>